<commit_message>
Update FYP Experiment Results.xlsx
</commit_message>
<xml_diff>
--- a/Difficulty in Learning/FYP Experiment Results.xlsx
+++ b/Difficulty in Learning/FYP Experiment Results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shearman Chua\Desktop\Difficulty in Learning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5122D9D-0CED-4609-BFEB-045C04FE12E9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{532EFC15-A45B-415E-B4D0-AC7A9E891643}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{B4CF8A72-EBF7-4C8F-A5F9-1796C5169378}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{B4CF8A72-EBF7-4C8F-A5F9-1796C5169378}"/>
   </bookViews>
   <sheets>
     <sheet name="Variation 1 Experiments" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="696" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="737" uniqueCount="52">
   <si>
     <t>Cyclic Stocks</t>
   </si>
@@ -313,7 +313,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -372,6 +372,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -691,20 +692,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DDF46CD2-B9AC-49C2-8DB4-A2F2A7816D99}">
-  <dimension ref="A2:AO52"/>
+  <dimension ref="A2:AO53"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A52" sqref="A52:T52"/>
+    <sheetView topLeftCell="D28" zoomScale="99" zoomScaleNormal="99" workbookViewId="0">
+      <selection activeCell="L56" sqref="L56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="34.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="41.5546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.88671875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="11.88671875" bestFit="1" customWidth="1"/>
-    <col min="7" max="9" width="16.21875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.88671875" customWidth="1"/>
+    <col min="7" max="9" width="16.21875" customWidth="1"/>
+    <col min="10" max="10" width="13.33203125" customWidth="1"/>
     <col min="11" max="11" width="18.21875" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="14.109375" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="12.77734375" bestFit="1" customWidth="1"/>
@@ -4913,189 +4915,209 @@
       <c r="A48" t="s">
         <v>33</v>
       </c>
+      <c r="B48" s="26"/>
+      <c r="C48" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="D48" s="23"/>
+      <c r="E48" s="23"/>
+      <c r="F48" s="23"/>
+      <c r="G48" s="23"/>
+      <c r="H48" s="23"/>
+      <c r="I48" s="23"/>
+      <c r="J48" s="23"/>
+      <c r="K48" s="23"/>
+      <c r="L48" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="M48" s="24"/>
+      <c r="N48" s="24"/>
+      <c r="O48" s="24"/>
+      <c r="P48" s="24"/>
+      <c r="Q48" s="24"/>
+      <c r="R48" s="24"/>
+      <c r="S48" s="24"/>
+      <c r="T48" s="24"/>
     </row>
     <row r="49" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A49" s="16" t="s">
-        <v>26</v>
-      </c>
-      <c r="B49" s="4">
-        <v>0.71378888888888892</v>
-      </c>
-      <c r="C49" s="4">
-        <v>0.71228888888888897</v>
-      </c>
-      <c r="D49" s="4">
-        <v>0.25423656565656549</v>
-      </c>
-      <c r="E49" s="4">
-        <v>0.28375408529741847</v>
-      </c>
-      <c r="F49" s="4">
-        <v>0.75098782320490465</v>
-      </c>
-      <c r="G49" s="4">
-        <v>0.56902568172568158</v>
-      </c>
-      <c r="H49" s="4">
-        <v>0.50472170428819962</v>
-      </c>
-      <c r="I49" s="4">
-        <v>0.84159525048232442</v>
-      </c>
-      <c r="J49" s="15">
-        <v>7.1539866506982241E-2</v>
-      </c>
-      <c r="K49" s="4">
-        <v>0.10158126594791406</v>
-      </c>
-      <c r="L49" s="4">
-        <v>0.72843333333333327</v>
-      </c>
-      <c r="M49" s="4">
-        <v>0.21373256373256355</v>
-      </c>
-      <c r="N49" s="4">
-        <v>0.25707070707070689</v>
-      </c>
-      <c r="O49" s="4">
-        <v>0.77818110078698277</v>
-      </c>
-      <c r="P49" s="4">
-        <v>0.56404717563573081</v>
-      </c>
-      <c r="Q49" s="4">
-        <v>0.56398921250453793</v>
-      </c>
-      <c r="R49" s="4">
-        <v>0.84795151426708448</v>
-      </c>
-      <c r="S49" s="13">
-        <v>0.10801694426235879</v>
-      </c>
-      <c r="T49" s="4">
-        <v>-6.1651181465506482E-3</v>
-      </c>
-      <c r="U49" s="19"/>
+      <c r="B49" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C49" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D49" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="E49" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="F49" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="G49" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="H49" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="I49" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="J49" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="K49" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="L49" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="M49" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="N49" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="O49" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="P49" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q49" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="R49" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="S49" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="T49" s="7" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="50" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A50" s="16" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B50" s="4">
-        <v>0.42711111111111111</v>
+        <v>0.71378888888888892</v>
       </c>
       <c r="C50" s="4">
-        <v>0.40614444444444447</v>
+        <v>0.71228888888888897</v>
       </c>
       <c r="D50" s="4">
-        <v>0.62401795735129051</v>
+        <v>0.25423656565656549</v>
       </c>
       <c r="E50" s="4">
-        <v>0.59455667789001099</v>
+        <v>0.28375408529741847</v>
       </c>
       <c r="F50" s="4">
-        <v>0.3876232167775428</v>
+        <v>0.75098782320490465</v>
       </c>
       <c r="G50" s="4">
-        <v>0.56968438159494417</v>
+        <v>0.56902568172568158</v>
       </c>
       <c r="H50" s="4">
-        <v>0.54198052453215861</v>
+        <v>0.50472170428819962</v>
       </c>
       <c r="I50" s="4">
-        <v>0.84594770159745236</v>
+        <v>0.84159525048232442</v>
       </c>
       <c r="J50" s="15">
-        <v>8.7028625554351133E-3</v>
+        <v>7.1539866506982241E-2</v>
       </c>
       <c r="K50" s="4">
         <v>0.10158126594791406</v>
       </c>
       <c r="L50" s="4">
-        <v>0.44571111111111111</v>
+        <v>0.72843333333333327</v>
       </c>
       <c r="M50" s="4">
-        <v>0.66484688151354798</v>
+        <v>0.21373256373256355</v>
       </c>
       <c r="N50" s="4">
-        <v>0.59332210998877655</v>
+        <v>0.25707070707070689</v>
       </c>
       <c r="O50" s="4">
-        <v>0.42749477217843929</v>
+        <v>0.77818110078698277</v>
       </c>
       <c r="P50" s="4">
-        <v>0.56104278279747477</v>
+        <v>0.56404717563573081</v>
       </c>
       <c r="Q50" s="4">
-        <v>0.60075953448666009</v>
+        <v>0.56398921250453793</v>
       </c>
       <c r="R50" s="4">
-        <v>0.86088859944806884</v>
-      </c>
-      <c r="S50" s="15">
-        <v>-0.19401299697546975</v>
+        <v>0.84795151426708448</v>
+      </c>
+      <c r="S50" s="13">
+        <v>0.10801694426235879</v>
       </c>
       <c r="T50" s="4">
         <v>-6.1651181465506482E-3</v>
       </c>
+      <c r="U50" s="19"/>
     </row>
     <row r="51" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A51" s="16" t="s">
-        <v>31</v>
-      </c>
-      <c r="B51" s="17">
-        <v>0.8482777777777778</v>
-      </c>
-      <c r="C51" s="17">
-        <v>0.8610000000000001</v>
-      </c>
-      <c r="D51" s="17">
-        <v>4.0404040404040317E-2</v>
-      </c>
-      <c r="E51" s="17">
-        <v>9.0796857463524006E-2</v>
-      </c>
-      <c r="F51" s="17">
-        <v>0.93394201856823522</v>
-      </c>
-      <c r="G51" s="17">
-        <v>0.54334215167548483</v>
-      </c>
-      <c r="H51" s="17">
-        <v>0.42549610882944183</v>
-      </c>
-      <c r="I51" s="17">
-        <v>0.83887170040939696</v>
+        <v>27</v>
+      </c>
+      <c r="B51" s="4">
+        <v>0.42711111111111111</v>
+      </c>
+      <c r="C51" s="4">
+        <v>0.40614444444444447</v>
+      </c>
+      <c r="D51" s="4">
+        <v>0.62401795735129051</v>
+      </c>
+      <c r="E51" s="4">
+        <v>0.59455667789001099</v>
+      </c>
+      <c r="F51" s="4">
+        <v>0.3876232167775428</v>
+      </c>
+      <c r="G51" s="4">
+        <v>0.56968438159494417</v>
+      </c>
+      <c r="H51" s="4">
+        <v>0.54198052453215861</v>
+      </c>
+      <c r="I51" s="4">
+        <v>0.84594770159745236</v>
       </c>
       <c r="J51" s="15">
-        <v>5.4242468055996376E-2</v>
+        <v>8.7028625554351133E-3</v>
       </c>
       <c r="K51" s="4">
         <v>0.10158126594791406</v>
       </c>
-      <c r="L51" s="17">
-        <v>0.86155555555555574</v>
-      </c>
-      <c r="M51" s="17">
-        <v>0.13192239858906513</v>
-      </c>
-      <c r="N51" s="17">
-        <v>5.353535353535345E-2</v>
-      </c>
-      <c r="O51" s="17">
-        <v>0.938147220735571</v>
-      </c>
-      <c r="P51" s="17">
-        <v>0.64135802469135783</v>
-      </c>
-      <c r="Q51" s="17">
-        <v>0.5242063492063489</v>
-      </c>
-      <c r="R51" s="17">
-        <v>0.8471415748328881</v>
-      </c>
-      <c r="S51" s="13">
-        <v>1.3255770145652586E-2</v>
+      <c r="L51" s="4">
+        <v>0.44571111111111111</v>
+      </c>
+      <c r="M51" s="4">
+        <v>0.66484688151354798</v>
+      </c>
+      <c r="N51" s="4">
+        <v>0.59332210998877655</v>
+      </c>
+      <c r="O51" s="4">
+        <v>0.42749477217843929</v>
+      </c>
+      <c r="P51" s="4">
+        <v>0.56104278279747477</v>
+      </c>
+      <c r="Q51" s="4">
+        <v>0.60075953448666009</v>
+      </c>
+      <c r="R51" s="4">
+        <v>0.86088859944806884</v>
+      </c>
+      <c r="S51" s="15">
+        <v>-0.19401299697546975</v>
       </c>
       <c r="T51" s="4">
         <v>-6.1651181465506482E-3</v>
@@ -5103,69 +5125,133 @@
     </row>
     <row r="52" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A52" s="16" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B52" s="17">
-        <v>0.76433333333333353</v>
+        <v>0.8482777777777778</v>
       </c>
       <c r="C52" s="17">
-        <v>0.75875555555555552</v>
+        <v>0.8610000000000001</v>
       </c>
       <c r="D52" s="17">
-        <v>0.18400673400673387</v>
+        <v>4.0404040404040317E-2</v>
       </c>
       <c r="E52" s="17">
-        <v>0.21778900112233432</v>
+        <v>9.0796857463524006E-2</v>
       </c>
       <c r="F52" s="17">
-        <v>0.81145083451513111</v>
+        <v>0.93394201856823522</v>
       </c>
       <c r="G52" s="17">
-        <v>0.59690494690494655</v>
+        <v>0.54334215167548483</v>
       </c>
       <c r="H52" s="17">
-        <v>0.57006480797131176</v>
+        <v>0.42549610882944183</v>
       </c>
       <c r="I52" s="17">
-        <v>0.84557985460587504</v>
-      </c>
-      <c r="J52" s="13">
-        <v>0.12529976883208691</v>
+        <v>0.83887170040939696</v>
+      </c>
+      <c r="J52" s="15">
+        <v>5.4242468055996376E-2</v>
       </c>
       <c r="K52" s="4">
         <v>0.10158126594791406</v>
       </c>
       <c r="L52" s="17">
-        <v>0.75675555555555551</v>
+        <v>0.86155555555555574</v>
       </c>
       <c r="M52" s="17">
-        <v>0.2018558601891933</v>
+        <v>0.13192239858906513</v>
       </c>
       <c r="N52" s="17">
-        <v>0.14031986531986515</v>
+        <v>5.353535353535345E-2</v>
       </c>
       <c r="O52" s="17">
-        <v>0.81490721686910694</v>
+        <v>0.938147220735571</v>
       </c>
       <c r="P52" s="17">
-        <v>0.58881106670153283</v>
+        <v>0.64135802469135783</v>
       </c>
       <c r="Q52" s="17">
-        <v>0.5424595807929139</v>
+        <v>0.5242063492063489</v>
       </c>
       <c r="R52" s="17">
-        <v>0.84540400121938564</v>
-      </c>
-      <c r="S52" s="15">
-        <v>-8.1819233839612815E-2</v>
+        <v>0.8471415748328881</v>
+      </c>
+      <c r="S52" s="13">
+        <v>1.3255770145652586E-2</v>
       </c>
       <c r="T52" s="4">
         <v>-6.1651181465506482E-3</v>
       </c>
-      <c r="U52" s="19"/>
+    </row>
+    <row r="53" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A53" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="B53" s="17">
+        <v>0.76433333333333353</v>
+      </c>
+      <c r="C53" s="17">
+        <v>0.75875555555555552</v>
+      </c>
+      <c r="D53" s="17">
+        <v>0.18400673400673387</v>
+      </c>
+      <c r="E53" s="17">
+        <v>0.21778900112233432</v>
+      </c>
+      <c r="F53" s="17">
+        <v>0.81145083451513111</v>
+      </c>
+      <c r="G53" s="17">
+        <v>0.59690494690494655</v>
+      </c>
+      <c r="H53" s="17">
+        <v>0.57006480797131176</v>
+      </c>
+      <c r="I53" s="17">
+        <v>0.84557985460587504</v>
+      </c>
+      <c r="J53" s="13">
+        <v>0.12529976883208691</v>
+      </c>
+      <c r="K53" s="4">
+        <v>0.10158126594791406</v>
+      </c>
+      <c r="L53" s="17">
+        <v>0.75675555555555551</v>
+      </c>
+      <c r="M53" s="17">
+        <v>0.2018558601891933</v>
+      </c>
+      <c r="N53" s="17">
+        <v>0.14031986531986515</v>
+      </c>
+      <c r="O53" s="17">
+        <v>0.81490721686910694</v>
+      </c>
+      <c r="P53" s="17">
+        <v>0.58881106670153283</v>
+      </c>
+      <c r="Q53" s="17">
+        <v>0.5424595807929139</v>
+      </c>
+      <c r="R53" s="17">
+        <v>0.84540400121938564</v>
+      </c>
+      <c r="S53" s="15">
+        <v>-8.1819233839612815E-2</v>
+      </c>
+      <c r="T53" s="4">
+        <v>-6.1651181465506482E-3</v>
+      </c>
+      <c r="U53" s="19"/>
     </row>
   </sheetData>
-  <mergeCells count="16">
+  <mergeCells count="18">
+    <mergeCell ref="C48:K48"/>
+    <mergeCell ref="L48:T48"/>
     <mergeCell ref="C37:K37"/>
     <mergeCell ref="L37:T37"/>
     <mergeCell ref="X37:AF37"/>
@@ -5190,10 +5276,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB0E4CD5-8A56-4C29-A8D4-3E4B1E27AB36}">
-  <dimension ref="A1:AM100"/>
+  <dimension ref="A1:AM101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="L107" sqref="L107"/>
+    <sheetView tabSelected="1" topLeftCell="A67" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="D102" sqref="D102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -12933,601 +13019,681 @@
       <c r="A89" t="s">
         <v>33</v>
       </c>
+      <c r="B89" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="C89" s="23"/>
+      <c r="D89" s="23"/>
+      <c r="E89" s="23"/>
+      <c r="F89" s="23"/>
+      <c r="G89" s="23"/>
+      <c r="H89" s="23"/>
+      <c r="I89" s="23"/>
+      <c r="J89" s="23"/>
+      <c r="K89" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="L89" s="24"/>
+      <c r="M89" s="24"/>
+      <c r="N89" s="24"/>
+      <c r="O89" s="24"/>
+      <c r="P89" s="24"/>
+      <c r="Q89" s="24"/>
+      <c r="R89" s="24"/>
+      <c r="S89" s="24"/>
     </row>
     <row r="90" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A90" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="B90" s="17">
-        <v>0.69372105598449663</v>
-      </c>
-      <c r="C90" s="17">
-        <v>0.27368125701459012</v>
-      </c>
-      <c r="D90" s="17">
-        <v>0.2810606060606059</v>
-      </c>
-      <c r="E90" s="17">
-        <v>0.73041042357855257</v>
-      </c>
-      <c r="F90" s="17">
-        <v>0.53724690143269727</v>
-      </c>
-      <c r="G90" s="17">
-        <v>0.50804027888625092</v>
-      </c>
-      <c r="H90" s="17">
-        <v>0.83553831138191959</v>
-      </c>
-      <c r="I90" s="15">
-        <v>-3.7663056200815978E-3</v>
-      </c>
-      <c r="J90" s="17">
-        <v>0.10158126594791406</v>
-      </c>
-      <c r="K90" s="17">
-        <v>0.71105641126632635</v>
-      </c>
-      <c r="L90" s="17">
-        <v>0.26518358185024821</v>
-      </c>
-      <c r="M90" s="17">
-        <v>0.28745791245791219</v>
-      </c>
-      <c r="N90" s="17">
-        <v>0.75442316184328917</v>
-      </c>
-      <c r="O90" s="17">
-        <v>0.58530123358339703</v>
-      </c>
-      <c r="P90" s="17">
-        <v>0.56956925370238021</v>
-      </c>
-      <c r="Q90" s="17">
-        <v>0.85025879330646992</v>
-      </c>
-      <c r="R90" s="13">
-        <v>0.10090376565911742</v>
-      </c>
-      <c r="S90" s="17">
-        <v>-6.1651181465506334E-3</v>
+      <c r="B90" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C90" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D90" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E90" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="F90" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="G90" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="H90" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="I90" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="J90" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="K90" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="L90" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="M90" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="N90" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="O90" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="P90" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q90" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="R90" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="S90" s="7" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="91" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A91" s="16" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B91" s="17">
-        <v>0.72921803593635504</v>
+        <v>0.69372105598449663</v>
       </c>
       <c r="C91" s="17">
-        <v>0.22081930415263734</v>
+        <v>0.27368125701459012</v>
       </c>
       <c r="D91" s="17">
-        <v>0.27760942760942747</v>
+        <v>0.2810606060606059</v>
       </c>
       <c r="E91" s="17">
-        <v>0.77197241357748836</v>
+        <v>0.73041042357855257</v>
       </c>
       <c r="F91" s="17">
-        <v>0.47649600125950287</v>
+        <v>0.53724690143269727</v>
       </c>
       <c r="G91" s="17">
-        <v>0.54978694850443155</v>
+        <v>0.50804027888625092</v>
       </c>
       <c r="H91" s="17">
-        <v>0.83723031968452011</v>
+        <v>0.83553831138191959</v>
       </c>
       <c r="I91" s="15">
-        <v>4.3741331783224098E-2</v>
+        <v>-3.7663056200815978E-3</v>
       </c>
       <c r="J91" s="17">
         <v>0.10158126594791406</v>
       </c>
       <c r="K91" s="17">
-        <v>0.74688865078820066</v>
+        <v>0.71105641126632635</v>
       </c>
       <c r="L91" s="17">
-        <v>0.25843354176687477</v>
+        <v>0.26518358185024821</v>
       </c>
       <c r="M91" s="17">
-        <v>0.19696969696969677</v>
+        <v>0.28745791245791219</v>
       </c>
       <c r="N91" s="17">
-        <v>0.80035288362275869</v>
+        <v>0.75442316184328917</v>
       </c>
       <c r="O91" s="17">
-        <v>0.54425770308123222</v>
+        <v>0.58530123358339703</v>
       </c>
       <c r="P91" s="17">
-        <v>0.54827571784093476</v>
+        <v>0.56956925370238021</v>
       </c>
       <c r="Q91" s="17">
-        <v>0.85062209803849043</v>
+        <v>0.85025879330646992</v>
       </c>
       <c r="R91" s="13">
-        <v>2.1208309756794219E-2</v>
+        <v>0.10090376565911742</v>
       </c>
       <c r="S91" s="17">
-        <v>-6.1651181465506482E-3</v>
+        <v>-6.1651181465506334E-3</v>
       </c>
     </row>
     <row r="92" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A92" s="16" t="s">
-        <v>50</v>
-      </c>
-      <c r="B92" s="4">
-        <v>0.71228888888888897</v>
-      </c>
-      <c r="C92" s="4">
-        <v>0.25423656565656549</v>
-      </c>
-      <c r="D92" s="4">
-        <v>0.28375408529741847</v>
-      </c>
-      <c r="E92" s="4">
-        <v>0.75098782320490465</v>
-      </c>
-      <c r="F92" s="4">
-        <v>0.56902568172568158</v>
-      </c>
-      <c r="G92" s="4">
-        <v>0.50472170428819962</v>
-      </c>
-      <c r="H92" s="4">
-        <v>0.84159525048232442</v>
+        <v>37</v>
+      </c>
+      <c r="B92" s="17">
+        <v>0.72921803593635504</v>
+      </c>
+      <c r="C92" s="17">
+        <v>0.22081930415263734</v>
+      </c>
+      <c r="D92" s="17">
+        <v>0.27760942760942747</v>
+      </c>
+      <c r="E92" s="17">
+        <v>0.77197241357748836</v>
+      </c>
+      <c r="F92" s="17">
+        <v>0.47649600125950287</v>
+      </c>
+      <c r="G92" s="17">
+        <v>0.54978694850443155</v>
+      </c>
+      <c r="H92" s="17">
+        <v>0.83723031968452011</v>
       </c>
       <c r="I92" s="15">
-        <v>7.1539866506982241E-2</v>
+        <v>4.3741331783224098E-2</v>
       </c>
       <c r="J92" s="17">
         <v>0.10158126594791406</v>
       </c>
-      <c r="K92" s="4">
-        <v>0.72843333333333327</v>
-      </c>
-      <c r="L92" s="4">
-        <v>0.21373256373256355</v>
-      </c>
-      <c r="M92" s="4">
-        <v>0.25707070707070689</v>
-      </c>
-      <c r="N92" s="4">
-        <v>0.77818110078698277</v>
-      </c>
-      <c r="O92" s="4">
-        <v>0.56404717563573081</v>
-      </c>
-      <c r="P92" s="4">
-        <v>0.56398921250453793</v>
-      </c>
-      <c r="Q92" s="4">
-        <v>0.84795151426708448</v>
+      <c r="K92" s="17">
+        <v>0.74688865078820066</v>
+      </c>
+      <c r="L92" s="17">
+        <v>0.25843354176687477</v>
+      </c>
+      <c r="M92" s="17">
+        <v>0.19696969696969677</v>
+      </c>
+      <c r="N92" s="17">
+        <v>0.80035288362275869</v>
+      </c>
+      <c r="O92" s="17">
+        <v>0.54425770308123222</v>
+      </c>
+      <c r="P92" s="17">
+        <v>0.54827571784093476</v>
+      </c>
+      <c r="Q92" s="17">
+        <v>0.85062209803849043</v>
       </c>
       <c r="R92" s="13">
-        <v>0.10801694426235879</v>
-      </c>
-      <c r="S92" s="4">
+        <v>2.1208309756794219E-2</v>
+      </c>
+      <c r="S92" s="17">
         <v>-6.1651181465506482E-3</v>
       </c>
     </row>
     <row r="93" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A93" s="16" t="s">
-        <v>41</v>
-      </c>
-      <c r="B93" s="17">
-        <v>0.69002718395656959</v>
-      </c>
-      <c r="C93" s="17">
-        <v>0.21257014590347911</v>
-      </c>
-      <c r="D93" s="17">
-        <v>0.27418630751964068</v>
-      </c>
-      <c r="E93" s="17">
-        <v>0.72835049666349816</v>
-      </c>
-      <c r="F93" s="17">
-        <v>0.49702218308356383</v>
-      </c>
-      <c r="G93" s="17">
-        <v>0.52517745106542868</v>
-      </c>
-      <c r="H93" s="17">
-        <v>0.83545443809679099</v>
+        <v>50</v>
+      </c>
+      <c r="B93" s="4">
+        <v>0.71228888888888897</v>
+      </c>
+      <c r="C93" s="4">
+        <v>0.25423656565656549</v>
+      </c>
+      <c r="D93" s="4">
+        <v>0.28375408529741847</v>
+      </c>
+      <c r="E93" s="4">
+        <v>0.75098782320490465</v>
+      </c>
+      <c r="F93" s="4">
+        <v>0.56902568172568158</v>
+      </c>
+      <c r="G93" s="4">
+        <v>0.50472170428819962</v>
+      </c>
+      <c r="H93" s="4">
+        <v>0.84159525048232442</v>
       </c>
       <c r="I93" s="15">
-        <v>1.5443463276334023E-2</v>
+        <v>7.1539866506982241E-2</v>
       </c>
       <c r="J93" s="17">
         <v>0.10158126594791406</v>
       </c>
-      <c r="K93" s="17">
-        <v>0.72045617633395664</v>
-      </c>
-      <c r="L93" s="17">
-        <v>0.23152958152958142</v>
-      </c>
-      <c r="M93" s="17">
-        <v>0.17906846240179553</v>
-      </c>
-      <c r="N93" s="17">
-        <v>0.77447147689231943</v>
-      </c>
-      <c r="O93" s="17">
-        <v>0.5451216724767447</v>
-      </c>
-      <c r="P93" s="17">
-        <v>0.59809362480169892</v>
-      </c>
-      <c r="Q93" s="17">
-        <v>0.84701477872937436</v>
+      <c r="K93" s="4">
+        <v>0.72843333333333327</v>
+      </c>
+      <c r="L93" s="4">
+        <v>0.21373256373256355</v>
+      </c>
+      <c r="M93" s="4">
+        <v>0.25707070707070689</v>
+      </c>
+      <c r="N93" s="4">
+        <v>0.77818110078698277</v>
+      </c>
+      <c r="O93" s="4">
+        <v>0.56404717563573081</v>
+      </c>
+      <c r="P93" s="4">
+        <v>0.56398921250453793</v>
+      </c>
+      <c r="Q93" s="4">
+        <v>0.84795151426708448</v>
       </c>
       <c r="R93" s="13">
-        <v>7.9142070727088953E-2</v>
-      </c>
-      <c r="S93" s="17">
+        <v>0.10801694426235879</v>
+      </c>
+      <c r="S93" s="4">
         <v>-6.1651181465506482E-3</v>
       </c>
     </row>
     <row r="94" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A94" s="16" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B94" s="17">
-        <v>0.75928165614604892</v>
+        <v>0.69002718395656959</v>
       </c>
       <c r="C94" s="17">
-        <v>0.13563131313131288</v>
+        <v>0.21257014590347911</v>
       </c>
       <c r="D94" s="17">
-        <v>0.19055555555555542</v>
+        <v>0.27418630751964068</v>
       </c>
       <c r="E94" s="17">
-        <v>0.81269821228306205</v>
+        <v>0.72835049666349816</v>
       </c>
       <c r="F94" s="17">
-        <v>0.5247751347161731</v>
+        <v>0.49702218308356383</v>
       </c>
       <c r="G94" s="17">
-        <v>0.43032828282828273</v>
+        <v>0.52517745106542868</v>
       </c>
       <c r="H94" s="17">
-        <v>0.82970756839456672</v>
-      </c>
-      <c r="I94" s="13">
-        <v>0.10433306471123398</v>
+        <v>0.83545443809679099</v>
+      </c>
+      <c r="I94" s="15">
+        <v>1.5443463276334023E-2</v>
       </c>
       <c r="J94" s="17">
         <v>0.10158126594791406</v>
       </c>
       <c r="K94" s="17">
-        <v>0.74846759438514687</v>
+        <v>0.72045617633395664</v>
       </c>
       <c r="L94" s="17">
-        <v>0.19334054834054823</v>
+        <v>0.23152958152958142</v>
       </c>
       <c r="M94" s="17">
-        <v>8.6590909090909093E-2</v>
+        <v>0.17906846240179553</v>
       </c>
       <c r="N94" s="17">
-        <v>0.80985833022465759</v>
+        <v>0.77447147689231943</v>
       </c>
       <c r="O94" s="17">
-        <v>0.59586704145527636</v>
+        <v>0.5451216724767447</v>
       </c>
       <c r="P94" s="17">
-        <v>0.5539436054141933</v>
+        <v>0.59809362480169892</v>
       </c>
       <c r="Q94" s="17">
-        <v>0.84919086713542069</v>
+        <v>0.84701477872937436</v>
       </c>
       <c r="R94" s="13">
-        <v>1.8475293531200337E-2</v>
+        <v>7.9142070727088953E-2</v>
       </c>
       <c r="S94" s="17">
         <v>-6.1651181465506482E-3</v>
       </c>
-      <c r="T94" s="19"/>
-    </row>
-    <row r="96" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A96" s="16" t="s">
+    </row>
+    <row r="95" spans="1:39" x14ac:dyDescent="0.3">
+      <c r="A95" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="B95" s="17">
+        <v>0.75928165614604892</v>
+      </c>
+      <c r="C95" s="17">
+        <v>0.13563131313131288</v>
+      </c>
+      <c r="D95" s="17">
+        <v>0.19055555555555542</v>
+      </c>
+      <c r="E95" s="17">
+        <v>0.81269821228306205</v>
+      </c>
+      <c r="F95" s="17">
+        <v>0.5247751347161731</v>
+      </c>
+      <c r="G95" s="17">
+        <v>0.43032828282828273</v>
+      </c>
+      <c r="H95" s="17">
+        <v>0.82970756839456672</v>
+      </c>
+      <c r="I95" s="13">
+        <v>0.10433306471123398</v>
+      </c>
+      <c r="J95" s="17">
+        <v>0.10158126594791406</v>
+      </c>
+      <c r="K95" s="17">
+        <v>0.74846759438514687</v>
+      </c>
+      <c r="L95" s="17">
+        <v>0.19334054834054823</v>
+      </c>
+      <c r="M95" s="17">
+        <v>8.6590909090909093E-2</v>
+      </c>
+      <c r="N95" s="17">
+        <v>0.80985833022465759</v>
+      </c>
+      <c r="O95" s="17">
+        <v>0.59586704145527636</v>
+      </c>
+      <c r="P95" s="17">
+        <v>0.5539436054141933</v>
+      </c>
+      <c r="Q95" s="17">
+        <v>0.84919086713542069</v>
+      </c>
+      <c r="R95" s="13">
+        <v>1.8475293531200337E-2</v>
+      </c>
+      <c r="S95" s="17">
+        <v>-6.1651181465506482E-3</v>
+      </c>
+      <c r="T95" s="19"/>
+    </row>
+    <row r="97" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A97" s="16" t="s">
         <v>44</v>
       </c>
-      <c r="B96" s="17">
+      <c r="B97" s="17">
         <v>0.76833240191141716</v>
       </c>
-      <c r="C96" s="17">
+      <c r="C97" s="17">
         <v>0.15297418630751944</v>
       </c>
-      <c r="D96" s="17">
+      <c r="D97" s="17">
         <v>0.1718294051627384</v>
       </c>
-      <c r="E96" s="17">
+      <c r="E97" s="17">
         <v>0.8248463656548477</v>
       </c>
-      <c r="F96" s="17">
+      <c r="F97" s="17">
         <v>0.57783224400871425</v>
       </c>
-      <c r="G96" s="17">
+      <c r="G97" s="17">
         <v>0.49639631031099868</v>
       </c>
-      <c r="H96" s="17">
+      <c r="H97" s="17">
         <v>0.83727261254667051</v>
       </c>
-      <c r="I96" s="15">
+      <c r="I97" s="15">
         <v>9.3256177715824257E-2</v>
-      </c>
-      <c r="J96" s="17">
-        <v>0.10158126594791406</v>
-      </c>
-      <c r="K96" s="17">
-        <v>0.79203322198655834</v>
-      </c>
-      <c r="L96" s="17">
-        <v>0.23145743145743131</v>
-      </c>
-      <c r="M96" s="17">
-        <v>0.11548821548821533</v>
-      </c>
-      <c r="N96" s="17">
-        <v>0.85284252917842318</v>
-      </c>
-      <c r="O96" s="17">
-        <v>0.54906830115558725</v>
-      </c>
-      <c r="P96" s="17">
-        <v>0.66804538054538021</v>
-      </c>
-      <c r="Q96" s="17">
-        <v>0.84566996108307146</v>
-      </c>
-      <c r="R96" s="13">
-        <v>0.20980769721853279</v>
-      </c>
-      <c r="S96" s="17">
-        <v>-6.1651181465506482E-3</v>
-      </c>
-      <c r="T96" s="19"/>
-    </row>
-    <row r="97" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A97" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="B97" s="17">
-        <v>0.75881003671222225</v>
-      </c>
-      <c r="C97" s="17">
-        <v>0.15521885521885509</v>
-      </c>
-      <c r="D97" s="17">
-        <v>0.14458473625140278</v>
-      </c>
-      <c r="E97" s="17">
-        <v>0.81574781892303705</v>
-      </c>
-      <c r="F97" s="17">
-        <v>0.47458732977583268</v>
-      </c>
-      <c r="G97" s="17">
-        <v>0.58599846504258257</v>
-      </c>
-      <c r="H97" s="17">
-        <v>0.834658284023862</v>
-      </c>
-      <c r="I97" s="15">
-        <v>3.6190839065523291E-2</v>
       </c>
       <c r="J97" s="17">
         <v>0.10158126594791406</v>
       </c>
       <c r="K97" s="17">
-        <v>0.75737749205695215</v>
+        <v>0.79203322198655834</v>
       </c>
       <c r="L97" s="17">
-        <v>0.17126022126022097</v>
+        <v>0.23145743145743131</v>
       </c>
       <c r="M97" s="17">
-        <v>0.13911335578002243</v>
+        <v>0.11548821548821533</v>
       </c>
       <c r="N97" s="17">
-        <v>0.8163863079475715</v>
+        <v>0.85284252917842318</v>
       </c>
       <c r="O97" s="17">
-        <v>0.56877458053928609</v>
+        <v>0.54906830115558725</v>
       </c>
       <c r="P97" s="17">
-        <v>0.57058951727143925</v>
+        <v>0.66804538054538021</v>
       </c>
       <c r="Q97" s="17">
-        <v>0.84537413761186064</v>
+        <v>0.84566996108307146</v>
       </c>
       <c r="R97" s="13">
-        <v>5.8887274155835577E-2</v>
+        <v>0.20980769721853279</v>
       </c>
       <c r="S97" s="17">
         <v>-6.1651181465506482E-3</v>
       </c>
-    </row>
-    <row r="98" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="T97" s="19"/>
+    </row>
+    <row r="98" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A98" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="B98" s="17">
+        <v>0.75881003671222225</v>
+      </c>
+      <c r="C98" s="17">
+        <v>0.15521885521885509</v>
+      </c>
+      <c r="D98" s="17">
+        <v>0.14458473625140278</v>
+      </c>
+      <c r="E98" s="17">
+        <v>0.81574781892303705</v>
+      </c>
+      <c r="F98" s="17">
+        <v>0.47458732977583268</v>
+      </c>
+      <c r="G98" s="17">
+        <v>0.58599846504258257</v>
+      </c>
+      <c r="H98" s="17">
+        <v>0.834658284023862</v>
+      </c>
+      <c r="I98" s="15">
+        <v>3.6190839065523291E-2</v>
+      </c>
+      <c r="J98" s="17">
+        <v>0.10158126594791406</v>
+      </c>
+      <c r="K98" s="17">
+        <v>0.75737749205695215</v>
+      </c>
+      <c r="L98" s="17">
+        <v>0.17126022126022097</v>
+      </c>
+      <c r="M98" s="17">
+        <v>0.13911335578002243</v>
+      </c>
+      <c r="N98" s="17">
+        <v>0.8163863079475715</v>
+      </c>
+      <c r="O98" s="17">
+        <v>0.56877458053928609</v>
+      </c>
+      <c r="P98" s="17">
+        <v>0.57058951727143925</v>
+      </c>
+      <c r="Q98" s="17">
+        <v>0.84537413761186064</v>
+      </c>
+      <c r="R98" s="13">
+        <v>5.8887274155835577E-2</v>
+      </c>
+      <c r="S98" s="17">
+        <v>-6.1651181465506482E-3</v>
+      </c>
+    </row>
+    <row r="99" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A99" s="16" t="s">
         <v>51</v>
       </c>
-      <c r="B98" s="17">
+      <c r="B99" s="17">
         <v>0.75875555555555552</v>
       </c>
-      <c r="C98" s="17">
+      <c r="C99" s="17">
         <v>0.18400673400673387</v>
       </c>
-      <c r="D98" s="17">
+      <c r="D99" s="17">
         <v>0.21778900112233432</v>
       </c>
-      <c r="E98" s="17">
+      <c r="E99" s="17">
         <v>0.81145083451513111</v>
       </c>
-      <c r="F98" s="17">
+      <c r="F99" s="17">
         <v>0.59690494690494655</v>
       </c>
-      <c r="G98" s="17">
+      <c r="G99" s="17">
         <v>0.57006480797131176</v>
       </c>
-      <c r="H98" s="17">
+      <c r="H99" s="17">
         <v>0.84557985460587504</v>
       </c>
-      <c r="I98" s="13">
+      <c r="I99" s="13">
         <v>0.12529976883208691</v>
       </c>
-      <c r="J98" s="4">
+      <c r="J99" s="4">
         <v>0.10158126594791406</v>
       </c>
-      <c r="K98" s="17">
+      <c r="K99" s="17">
         <v>0.75675555555555551</v>
       </c>
-      <c r="L98" s="17">
+      <c r="L99" s="17">
         <v>0.2018558601891933</v>
       </c>
-      <c r="M98" s="17">
+      <c r="M99" s="17">
         <v>0.14031986531986515</v>
       </c>
-      <c r="N98" s="17">
+      <c r="N99" s="17">
         <v>0.81490721686910694</v>
       </c>
-      <c r="O98" s="17">
+      <c r="O99" s="17">
         <v>0.58881106670153283</v>
       </c>
-      <c r="P98" s="17">
+      <c r="P99" s="17">
         <v>0.5424595807929139</v>
       </c>
-      <c r="Q98" s="17">
+      <c r="Q99" s="17">
         <v>0.84540400121938564</v>
       </c>
-      <c r="R98" s="15">
+      <c r="R99" s="15">
         <v>-8.1819233839612815E-2</v>
       </c>
-      <c r="S98" s="4">
+      <c r="S99" s="4">
         <v>-6.1651181465506482E-3</v>
       </c>
     </row>
-    <row r="99" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A99" s="16" t="s">
+    <row r="100" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A100" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="B99" s="17">
+      <c r="B100" s="17">
         <v>0.77130791213777283</v>
       </c>
-      <c r="C99" s="17">
+      <c r="C100" s="17">
         <v>0.13622334455667764</v>
       </c>
-      <c r="D99" s="17">
+      <c r="D100" s="17">
         <v>0.16843434343434333</v>
       </c>
-      <c r="E99" s="17">
+      <c r="E100" s="17">
         <v>0.82903604165415146</v>
       </c>
-      <c r="F99" s="17">
+      <c r="F100" s="17">
         <v>0.49014279112318299</v>
       </c>
-      <c r="G99" s="17">
+      <c r="G100" s="17">
         <v>0.57185843946713488</v>
       </c>
-      <c r="H99" s="17">
+      <c r="H100" s="17">
         <v>0.84257629140134449</v>
       </c>
-      <c r="I99" s="15">
+      <c r="I100" s="15">
         <v>3.3771417301557811E-2</v>
-      </c>
-      <c r="J99" s="17">
-        <v>0.10158126594791406</v>
-      </c>
-      <c r="K99" s="17">
-        <v>0.8061084018813236</v>
-      </c>
-      <c r="L99" s="17">
-        <v>0.14626022126022098</v>
-      </c>
-      <c r="M99" s="17">
-        <v>4.2592592592592592E-2</v>
-      </c>
-      <c r="N99" s="17">
-        <v>0.87665974614337072</v>
-      </c>
-      <c r="O99" s="17">
-        <v>0.48377933794600431</v>
-      </c>
-      <c r="P99" s="17">
-        <v>0.46714609866783757</v>
-      </c>
-      <c r="Q99" s="17">
-        <v>0.78242253220380231</v>
-      </c>
-      <c r="R99" s="13">
-        <v>-6.1058294273601084E-3</v>
-      </c>
-      <c r="S99" s="17">
-        <v>-6.1651181465506482E-3</v>
-      </c>
-    </row>
-    <row r="100" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A100" s="16" t="s">
-        <v>49</v>
-      </c>
-      <c r="B100" s="17">
-        <v>0.76836323738098122</v>
-      </c>
-      <c r="C100" s="17">
-        <v>0.19363075196408522</v>
-      </c>
-      <c r="D100" s="17">
-        <v>0.15701459034792353</v>
-      </c>
-      <c r="E100" s="17">
-        <v>0.82478117757095626</v>
-      </c>
-      <c r="F100" s="17">
-        <v>0.53830933040259787</v>
-      </c>
-      <c r="G100" s="17">
-        <v>0.53823462479376416</v>
-      </c>
-      <c r="H100" s="17">
-        <v>0.84288931226660868</v>
-      </c>
-      <c r="I100" s="15">
-        <v>2.8420755985839811E-2</v>
       </c>
       <c r="J100" s="17">
         <v>0.10158126594791406</v>
       </c>
       <c r="K100" s="17">
-        <v>0.76085477405124202</v>
+        <v>0.8061084018813236</v>
       </c>
       <c r="L100" s="17">
-        <v>0.18528138528138513</v>
+        <v>0.14626022126022098</v>
       </c>
       <c r="M100" s="17">
-        <v>0.17673961840628491</v>
+        <v>4.2592592592592592E-2</v>
       </c>
       <c r="N100" s="17">
-        <v>0.81808753161787218</v>
+        <v>0.87665974614337072</v>
       </c>
       <c r="O100" s="17">
-        <v>0.53189244154156379</v>
+        <v>0.48377933794600431</v>
       </c>
       <c r="P100" s="17">
-        <v>0.56207504838336453</v>
+        <v>0.46714609866783757</v>
       </c>
       <c r="Q100" s="17">
-        <v>0.84475855781486486</v>
+        <v>0.78242253220380231</v>
       </c>
       <c r="R100" s="13">
-        <v>1.2828258380139519E-2</v>
+        <v>-6.1058294273601084E-3</v>
       </c>
       <c r="S100" s="17">
         <v>-6.1651181465506482E-3</v>
       </c>
     </row>
+    <row r="101" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A101" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="B101" s="17">
+        <v>0.76836323738098122</v>
+      </c>
+      <c r="C101" s="17">
+        <v>0.19363075196408522</v>
+      </c>
+      <c r="D101" s="17">
+        <v>0.15701459034792353</v>
+      </c>
+      <c r="E101" s="17">
+        <v>0.82478117757095626</v>
+      </c>
+      <c r="F101" s="17">
+        <v>0.53830933040259787</v>
+      </c>
+      <c r="G101" s="17">
+        <v>0.53823462479376416</v>
+      </c>
+      <c r="H101" s="17">
+        <v>0.84288931226660868</v>
+      </c>
+      <c r="I101" s="15">
+        <v>2.8420755985839811E-2</v>
+      </c>
+      <c r="J101" s="17">
+        <v>0.10158126594791406</v>
+      </c>
+      <c r="K101" s="17">
+        <v>0.76085477405124202</v>
+      </c>
+      <c r="L101" s="17">
+        <v>0.18528138528138513</v>
+      </c>
+      <c r="M101" s="17">
+        <v>0.17673961840628491</v>
+      </c>
+      <c r="N101" s="17">
+        <v>0.81808753161787218</v>
+      </c>
+      <c r="O101" s="17">
+        <v>0.53189244154156379</v>
+      </c>
+      <c r="P101" s="17">
+        <v>0.56207504838336453</v>
+      </c>
+      <c r="Q101" s="17">
+        <v>0.84475855781486486</v>
+      </c>
+      <c r="R101" s="13">
+        <v>1.2828258380139519E-2</v>
+      </c>
+      <c r="S101" s="17">
+        <v>-6.1651181465506482E-3</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="32">
+  <mergeCells count="34">
+    <mergeCell ref="B89:J89"/>
+    <mergeCell ref="K89:S89"/>
     <mergeCell ref="B69:J69"/>
     <mergeCell ref="K69:S69"/>
     <mergeCell ref="V69:AD69"/>

</xml_diff>